<commit_message>
Bicubic adjustable dimming curve
</commit_message>
<xml_diff>
--- a/doc/log-dimming-curve.xlsx
+++ b/doc/log-dimming-curve.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" state="visible" r:id="rId2"/>
@@ -284,7 +284,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -299,7 +299,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Log!$B$6:$B$6</c:f>
+              <c:f>X3!$B$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -318,8 +318,6 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -329,7 +327,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Log!$B$7:$B$262</c:f>
+              <c:f>X3!$B$8:$B$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -1110,7 +1108,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Log!$C$6:$C$6</c:f>
+              <c:f>X3!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1129,8 +1127,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="outEnd"/>
+            <c:numFmt formatCode="0" sourceLinked="1"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1140,7 +1137,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Log!$C$7:$C$262</c:f>
+              <c:f>X3!$C$8:$C$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -1148,769 +1145,769 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.0189530180857</c:v>
+                  <c:v>36.0214834656354</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.0383224012084</c:v>
+                  <c:v>36.0430441956713</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.0581172961878</c:v>
+                  <c:v>36.0647594545084</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0783470507838</c:v>
+                  <c:v>36.0867065065473</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.0990212181103</c:v>
+                  <c:v>36.1089626161883</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.1201495611466</c:v>
+                  <c:v>36.1316050478323</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.1417420573477</c:v>
+                  <c:v>36.1547110658796</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.1638089033561</c:v>
+                  <c:v>36.178357934731</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.186360519817</c:v>
+                  <c:v>36.2026229187869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.2094075562988</c:v>
+                  <c:v>36.2275832824479</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.2329608963231</c:v>
+                  <c:v>36.2533162901147</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.257031662503</c:v>
+                  <c:v>36.2798992061877</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.2816312217967</c:v>
+                  <c:v>36.3074092950675</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.3067711908745</c:v>
+                  <c:v>36.3359238211548</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.332463441605</c:v>
+                  <c:v>36.36552004885</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36.3587201066613</c:v>
+                  <c:v>36.3962752425538</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36.38555358525</c:v>
+                  <c:v>36.4282666666667</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.4129765489673</c:v>
+                  <c:v>36.4615715855893</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.4410019477821</c:v>
+                  <c:v>36.4962672637221</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.469643016152</c:v>
+                  <c:v>36.5324309654658</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.4989132792724</c:v>
+                  <c:v>36.5701399552208</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.5288265594643</c:v>
+                  <c:v>36.6094714973879</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.5593969827008</c:v>
+                  <c:v>36.6505028563675</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.5906389852784</c:v>
+                  <c:v>36.6933112965601</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.622567320634</c:v>
+                  <c:v>36.7379740823665</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.6551970663122</c:v>
+                  <c:v>36.7845684781871</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36.6885436310848</c:v>
+                  <c:v>36.8331717484225</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>36.7226227622281</c:v>
+                  <c:v>36.8838611574734</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>36.7574505529585</c:v>
+                  <c:v>36.9367139697401</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>36.7930434500327</c:v>
+                  <c:v>36.9918074496235</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>36.8294182615142</c:v>
+                  <c:v>37.0492188615238</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>36.8665921647106</c:v>
+                  <c:v>37.1090254698419</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>36.9045827142851</c:v>
+                  <c:v>37.1713045389782</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>36.9434078505468</c:v>
+                  <c:v>37.2361333333333</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36.983085907922</c:v>
+                  <c:v>37.3035891173078</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37.0236356236128</c:v>
+                  <c:v>37.3737491553023</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.0650761464455</c:v>
+                  <c:v>37.4466907117172</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>37.1074270459126</c:v>
+                  <c:v>37.5224910509533</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>37.1507083214147</c:v>
+                  <c:v>37.6012274374109</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>37.1949404117047</c:v>
+                  <c:v>37.6829771354909</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>37.2401442045395</c:v>
+                  <c:v>37.7678174095936</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>37.2863410465437</c:v>
+                  <c:v>37.8558255241197</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>37.3335527532908</c:v>
+                  <c:v>37.9470787434697</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>37.3818016196043</c:v>
+                  <c:v>38.0416543320442</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>37.4311104300867</c:v>
+                  <c:v>38.1396295542438</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>37.4815024698785</c:v>
+                  <c:v>38.2410816744691</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>37.533001535655</c:v>
+                  <c:v>38.3460879571206</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>37.5856319468627</c:v>
+                  <c:v>38.4547256665988</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>37.6394185572047</c:v>
+                  <c:v>38.5670720673044</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>37.694386766377</c:v>
+                  <c:v>38.683204423638</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>37.7505625320626</c:v>
+                  <c:v>38.8032</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>37.8079723821904</c:v>
+                  <c:v>38.9271360607911</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>37.8666434274618</c:v>
+                  <c:v>39.0550898704118</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>37.9266033741533</c:v>
+                  <c:v>39.1871386932628</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>37.9878805372007</c:v>
+                  <c:v>39.3233597937445</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>38.0505038535698</c:v>
+                  <c:v>39.4638304362575</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>38.1145028959215</c:v>
+                  <c:v>39.6086278852025</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>38.1799078865769</c:v>
+                  <c:v>39.75782940498</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>38.2467497117894</c:v>
+                  <c:v>39.9115122599905</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>38.3150599363298</c:v>
+                  <c:v>40.0697537146346</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>38.3848708183925</c:v>
+                  <c:v>40.232631033313</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>38.4562153248285</c:v>
+                  <c:v>40.4002214804261</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>38.5291271467136</c:v>
+                  <c:v>40.5726023203745</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>38.6036407152582</c:v>
+                  <c:v>40.7498508175589</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>38.6797912180671</c:v>
+                  <c:v>40.9320442363797</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>38.7576146157557</c:v>
+                  <c:v>41.1192598412375</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>38.8371476589319</c:v>
+                  <c:v>41.311574896533</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>38.9184279055512</c:v>
+                  <c:v>41.5090666666667</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>39.0014937386521</c:v>
+                  <c:v>41.7118124160391</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>39.0863843844823</c:v>
+                  <c:v>41.9198894090508</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>39.1731399310224</c:v>
+                  <c:v>42.1333749101025</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>39.2618013469164</c:v>
+                  <c:v>42.3523461835945</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>39.3524105008188</c:v>
+                  <c:v>42.5768804939277</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>39.4450101811658</c:v>
+                  <c:v>42.8070551055024</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>39.5396441163817</c:v>
+                  <c:v>43.0429472827193</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>39.6363569955288</c:v>
+                  <c:v>43.284634289979</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>39.7351944894106</c:v>
+                  <c:v>43.5321933916819</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>39.8362032721392</c:v>
+                  <c:v>43.7857018522288</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>39.9394310431766</c:v>
+                  <c:v>44.0452369360201</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>40.0449265498589</c:v>
+                  <c:v>44.3108759074564</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>40.1527396104175</c:v>
+                  <c:v>44.5826960309383</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>40.2629211375037</c:v>
+                  <c:v>44.8607745708664</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>40.3755231622321</c:v>
+                  <c:v>45.1451887916412</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>40.4905988587508</c:v>
+                  <c:v>45.4360159576634</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>40.6082025693518</c:v>
+                  <c:v>45.7333333333333</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>40.7283898301335</c:v>
+                  <c:v>46.0372181830518</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>40.8512173972264</c:v>
+                  <c:v>46.3477477712192</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>40.9767432735949</c:v>
+                  <c:v>46.6649993622363</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>41.1050267364284</c:v>
+                  <c:v>46.9890502205034</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>41.2361283651334</c:v>
+                  <c:v>47.3199776104213</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>41.3701100699416</c:v>
+                  <c:v>47.6578587963905</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>41.507035121145</c:v>
+                  <c:v>48.0027710428116</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>41.6469681789749</c:v>
+                  <c:v>48.3547916140851</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>41.7899753241359</c:v>
+                  <c:v>48.7139977746116</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>41.9361240890115</c:v>
+                  <c:v>49.0804667887916</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>42.0854834895547</c:v>
+                  <c:v>49.4542759210258</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>42.23812405788</c:v>
+                  <c:v>49.8355024357148</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>42.3941178755702</c:v>
+                  <c:v>50.224223597259</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>42.5535386077159</c:v>
+                  <c:v>50.620516670059</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>42.7164615377026</c:v>
+                  <c:v>51.0244589185155</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>42.8829636027612</c:v>
+                  <c:v>51.436127607029</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>43.053123430301</c:v>
+                  <c:v>51.8556</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>43.2270213750392</c:v>
+                  <c:v>52.2829533618292</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>43.4047395569474</c:v>
+                  <c:v>52.718264956917</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>43.5863619000307</c:v>
+                  <c:v>53.1616120496642</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>43.7719741719598</c:v>
+                  <c:v>53.6130719044711</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>43.9616640245728</c:v>
+                  <c:v>54.0727217857385</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>44.1555210352668</c:v>
+                  <c:v>54.5406389578669</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>44.3536367492999</c:v>
+                  <c:v>55.0169006852568</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>44.5561047230209</c:v>
+                  <c:v>55.5015842323089</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>44.76302056805</c:v>
+                  <c:v>55.9947668634236</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>44.9744819964291</c:v>
+                  <c:v>56.4965258430016</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>45.1905888667651</c:v>
+                  <c:v>57.0069384354434</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>45.4114432313857</c:v>
+                  <c:v>57.5260819051496</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>45.6371493845316</c:v>
+                  <c:v>58.0540335165208</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>45.8678139116078</c:v>
+                  <c:v>58.5908705339575</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>46.1035457395164</c:v>
+                  <c:v>59.1366702218604</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>46.3444561880951</c:v>
+                  <c:v>59.6915098446299</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>46.5906590226859</c:v>
+                  <c:v>60.2554666666667</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>46.842270507859</c:v>
+                  <c:v>60.8286179523713</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>47.0994094623157</c:v>
+                  <c:v>61.4110409661442</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>47.3621973149991</c:v>
+                  <c:v>62.0028129723862</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>47.630758162436</c:v>
+                  <c:v>62.6040112354977</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>47.9052188273395</c:v>
+                  <c:v>63.2147130198792</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>48.1857089184983</c:v>
+                  <c:v>63.8349955899315</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>48.472360891982</c:v>
+                  <c:v>64.464936210055</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>48.7653101136914</c:v>
+                  <c:v>65.1046121446503</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>49.0646949232817</c:v>
+                  <c:v>65.7541006581179</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>49.3706566994912</c:v>
+                  <c:v>66.4134790148585</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>49.6833399269049</c:v>
+                  <c:v>67.0828244792727</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>50.002892264184</c:v>
+                  <c:v>67.7622143157609</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>50.3294646137953</c:v>
+                  <c:v>68.4517257887238</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>50.6632111932718</c:v>
+                  <c:v>69.1514361625619</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>51.0042896080393</c:v>
+                  <c:v>69.8614227016758</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>51.3528609258421</c:v>
+                  <c:v>70.5817626704661</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>51.7090897528043</c:v>
+                  <c:v>71.3125333333333</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>52.073144311162</c:v>
+                  <c:v>72.0538119546781</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>52.445196518703</c:v>
+                  <c:v>72.8056757989009</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>52.8254220699517</c:v>
+                  <c:v>73.5682021304023</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>53.2140005191373</c:v>
+                  <c:v>74.341468213583</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>53.611115364985</c:v>
+                  <c:v>75.1255513128435</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>54.0169541373697</c:v>
+                  <c:v>75.9205286925843</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>54.4317084858735</c:v>
+                  <c:v>76.7264776172061</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>54.8555742702883</c:v>
+                  <c:v>77.5434753511093</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>55.288751653107</c:v>
+                  <c:v>78.3715991586946</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>55.7314451940466</c:v>
+                  <c:v>79.2109263043626</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>56.1838639466471</c:v>
+                  <c:v>80.0615340525137</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>56.6462215569934</c:v>
+                  <c:v>80.9234996675487</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>57.1187363646057</c:v>
+                  <c:v>81.796900413868</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>57.6016315055457</c:v>
+                  <c:v>82.6818135558722</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>58.0951350177885</c:v>
+                  <c:v>83.5783163579619</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>58.5994799489095</c:v>
+                  <c:v>84.4864860845376</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>59.1149044661362</c:v>
+                  <c:v>85.4064</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>59.6416519688183</c:v>
+                  <c:v>86.3381353687496</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>60.1799712033685</c:v>
+                  <c:v>87.2817694551869</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>60.7301163807278</c:v>
+                  <c:v>88.2373795237126</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>61.2923472964123</c:v>
+                  <c:v>89.2050428387272</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>61.8669294531964</c:v>
+                  <c:v>90.1848366646313</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>62.4541341864913</c:v>
+                  <c:v>91.1768382658254</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>63.0542387924779</c:v>
+                  <c:v>92.1811249067101</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>63.667526659055</c:v>
+                  <c:v>93.197773851686</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>64.2942873996634</c:v>
+                  <c:v>94.2268623651537</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>64.9348169900504</c:v>
+                  <c:v>95.2684677115137</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>65.5894179080389</c:v>
+                  <c:v>96.3226671551666</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>66.2583992763665</c:v>
+                  <c:v>97.3895379605129</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>66.9420770086626</c:v>
+                  <c:v>98.4691573919533</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>67.6407739586333</c:v>
+                  <c:v>99.5616027138883</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>68.3548200725219</c:v>
+                  <c:v>100.666951190719</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>69.0845525449205</c:v>
+                  <c:v>101.785280086844</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>69.8303159780033</c:v>
+                  <c:v>102.916666666667</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>70.5924625442583</c:v>
+                  <c:v>104.061188194586</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>71.3713521527944</c:v>
+                  <c:v>105.218921935002</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>72.1673526193011</c:v>
+                  <c:v>106.389945152317</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>72.9808398397427</c:v>
+                  <c:v>107.57433511093</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>73.8121979678679</c:v>
+                  <c:v>108.772169075243</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>74.661819596619</c:v>
+                  <c:v>109.983524309655</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>75.5301059435266</c:v>
+                  <c:v>111.208478078567</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>76.4174670401766</c:v>
+                  <c:v>112.44710764638</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>77.3243219258398</c:v>
+                  <c:v>113.699490277495</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>78.2510988453554</c:v>
+                  <c:v>114.965703236312</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>79.1982354513611</c:v>
+                  <c:v>116.245823787231</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>80.1661790109667</c:v>
+                  <c:v>117.539929194654</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>81.1553866169665</c:v>
+                  <c:v>118.84809672298</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>82.1663254036936</c:v>
+                  <c:v>120.17040363661</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>83.1994727676146</c:v>
+                  <c:v>121.506927199946</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>84.2553165927709</c:v>
+                  <c:v>122.857744677387</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>85.3343554811729</c:v>
+                  <c:v>124.222933333333</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>86.4370989882549</c:v>
+                  <c:v>125.602570432187</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>87.5640678635032</c:v>
+                  <c:v>126.996733238347</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>88.7157942963698</c:v>
+                  <c:v>128.405499016216</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>89.892822167589</c:v>
+                  <c:v>129.828945030192</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>91.0957073060141</c:v>
+                  <c:v>131.267148544677</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>92.3250177510975</c:v>
+                  <c:v>132.720186824072</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>93.5813340211361</c:v>
+                  <c:v>134.188137132777</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>94.8652493874103</c:v>
+                  <c:v>135.671076735192</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>96.1773701543443</c:v>
+                  <c:v>137.169082895719</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>97.5183159458225</c:v>
+                  <c:v>138.682232878757</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>98.8887199977947</c:v>
+                  <c:v>140.210603948708</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>100.289229457309</c:v>
+                  <c:v>141.754273369971</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>101.720505688117</c:v>
+                  <c:v>143.313318406948</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>103.183224582986</c:v>
+                  <c:v>144.887816324038</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>104.67807688288</c:v>
+                  <c:v>146.477844385643</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>106.205768503148</c:v>
+                  <c:v>148.083479856164</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>107.767020866878</c:v>
+                  <c:v>149.7048</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>109.362571245576</c:v>
+                  <c:v>151.341882081552</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>110.993173107328</c:v>
+                  <c:v>152.994803365222</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>112.659596472612</c:v>
+                  <c:v>154.663641115408</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>114.362628277924</c:v>
+                  <c:v>156.348472596513</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>116.103072747393</c:v>
+                  <c:v>158.049375072936</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>117.881751772564</c:v>
+                  <c:v>159.766425809078</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>119.699505300516</c:v>
+                  <c:v>161.49970206934</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>121.557191730514</c:v>
+                  <c:v>163.249281118122</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>123.455688319371</c:v>
+                  <c:v>165.015240219825</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>125.395891595714</c:v>
+                  <c:v>166.797656638849</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>127.378717783355</c:v>
+                  <c:v>168.596607639596</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>129.405103233958</c:v>
+                  <c:v>170.412170486464</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>131.476004869216</c:v>
+                  <c:v>172.244422443856</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>133.592400632735</c:v>
+                  <c:v>174.093440776172</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>135.755289951853</c:v>
+                  <c:v>175.959302747812</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>137.965694209595</c:v>
+                  <c:v>177.842085623177</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>140.22465722701</c:v>
+                  <c:v>179.741866666667</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>142.533245756086</c:v>
+                  <c:v>181.658723142683</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>144.892549983511</c:v>
+                  <c:v>183.592732315625</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>147.303684045489</c:v>
+                  <c:v>185.543971449895</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>149.767786553868</c:v>
+                  <c:v>187.512517809892</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>152.286021133832</c:v>
+                  <c:v>189.498448660018</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>154.859576973397</c:v>
+                  <c:v>191.501841264672</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>157.489669384984</c:v>
+                  <c:v>193.522772888256</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>160.177540379327</c:v>
+                  <c:v>195.561320795169</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>162.924459251987</c:v>
+                  <c:v>197.617562249813</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>165.731723182754</c:v>
+                  <c:v>199.691574516589</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>168.600657848218</c:v>
+                  <c:v>201.783434859895</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>171.532618047788</c:v>
+                  <c:v>203.893220544135</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>174.528988343475</c:v>
+                  <c:v>206.021008833706</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>177.591183713723</c:v>
+                  <c:v>208.166876993012</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>180.720650221606</c:v>
+                  <c:v>210.330902286451</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>183.918865697705</c:v>
+                  <c:v>212.513161978425</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>187.18734043798</c:v>
+                  <c:v>214.713733333333</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>190.527617916985</c:v>
+                  <c:v>216.932693615578</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>193.941275516741</c:v>
+                  <c:v>219.170120089558</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>197.429925271623</c:v>
+                  <c:v>221.426090019676</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>200.995214629616</c:v>
+                  <c:v>223.70068067033</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>204.638827230286</c:v>
+                  <c:v>225.993969305923</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>208.362483699853</c:v>
+                  <c:v>228.306033190854</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>212.167942463716</c:v>
+                  <c:v>230.636949589524</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>216.057000576842</c:v>
+                  <c:v>232.986795766334</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>220.031494572388</c:v>
+                  <c:v>235.355648985684</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>224.093301328969</c:v>
+                  <c:v>237.743586511975</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>228.244338956978</c:v>
+                  <c:v>240.150685609607</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>232.486567704377</c:v>
+                  <c:v>242.577023542981</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>236.821990882386</c:v>
+                  <c:v>245.022677576498</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>241.252655811509</c:v>
+                  <c:v>247.487724974557</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>245.780654788341</c:v>
+                  <c:v>249.97224300156</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>250.408126073617</c:v>
+                  <c:v>252.476308921908</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>255.137254901961</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1918,11 +1915,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="31123728"/>
-        <c:axId val="88808483"/>
+        <c:axId val="36811195"/>
+        <c:axId val="96435088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31123728"/>
+        <c:axId val="36811195"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,14 +1947,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88808483"/>
+        <c:crossAx val="96435088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88808483"/>
+        <c:axId val="96435088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1972,7 +1969,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1994,7 +1991,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31123728"/>
+        <c:crossAx val="36811195"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2041,7 +2038,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2056,7 +2053,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>X3!$B$7</c:f>
+              <c:f>Log!$B$6:$B$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2075,6 +2072,8 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2084,7 +2083,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>X3!$B$8:$B$263</c:f>
+              <c:f>Log!$B$7:$B$262</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -2865,7 +2864,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>X3!$C$7</c:f>
+              <c:f>Log!$C$6:$C$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2884,7 +2883,8 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="0" sourceLinked="1"/>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2894,7 +2894,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>X3!$C$8:$C$263</c:f>
+              <c:f>Log!$C$7:$C$262</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -2902,769 +2902,769 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.0214834656354</c:v>
+                  <c:v>36.0189530180857</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.0430441956713</c:v>
+                  <c:v>36.0383224012084</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.0647594545084</c:v>
+                  <c:v>36.0581172961878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.0867065065473</c:v>
+                  <c:v>36.0783470507838</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.1089626161883</c:v>
+                  <c:v>36.0990212181103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.1316050478323</c:v>
+                  <c:v>36.1201495611466</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.1547110658796</c:v>
+                  <c:v>36.1417420573477</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.178357934731</c:v>
+                  <c:v>36.1638089033561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.2026229187869</c:v>
+                  <c:v>36.186360519817</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.2275832824479</c:v>
+                  <c:v>36.2094075562988</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.2533162901147</c:v>
+                  <c:v>36.2329608963231</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.2798992061877</c:v>
+                  <c:v>36.257031662503</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.3074092950675</c:v>
+                  <c:v>36.2816312217967</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.3359238211548</c:v>
+                  <c:v>36.3067711908745</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.36552004885</c:v>
+                  <c:v>36.332463441605</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36.3962752425538</c:v>
+                  <c:v>36.3587201066613</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36.4282666666667</c:v>
+                  <c:v>36.38555358525</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.4615715855893</c:v>
+                  <c:v>36.4129765489673</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.4962672637221</c:v>
+                  <c:v>36.4410019477821</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.5324309654658</c:v>
+                  <c:v>36.469643016152</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.5701399552208</c:v>
+                  <c:v>36.4989132792724</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.6094714973879</c:v>
+                  <c:v>36.5288265594643</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.6505028563675</c:v>
+                  <c:v>36.5593969827008</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.6933112965601</c:v>
+                  <c:v>36.5906389852784</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.7379740823665</c:v>
+                  <c:v>36.622567320634</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.7845684781871</c:v>
+                  <c:v>36.6551970663122</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36.8331717484225</c:v>
+                  <c:v>36.6885436310848</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>36.8838611574734</c:v>
+                  <c:v>36.7226227622281</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>36.9367139697401</c:v>
+                  <c:v>36.7574505529585</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>36.9918074496235</c:v>
+                  <c:v>36.7930434500327</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>37.0492188615238</c:v>
+                  <c:v>36.8294182615142</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37.1090254698419</c:v>
+                  <c:v>36.8665921647106</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>37.1713045389782</c:v>
+                  <c:v>36.9045827142851</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>37.2361333333333</c:v>
+                  <c:v>36.9434078505468</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>37.3035891173078</c:v>
+                  <c:v>36.983085907922</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>37.3737491553023</c:v>
+                  <c:v>37.0236356236128</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>37.4466907117172</c:v>
+                  <c:v>37.0650761464455</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>37.5224910509533</c:v>
+                  <c:v>37.1074270459126</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>37.6012274374109</c:v>
+                  <c:v>37.1507083214147</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>37.6829771354909</c:v>
+                  <c:v>37.1949404117047</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>37.7678174095936</c:v>
+                  <c:v>37.2401442045395</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>37.8558255241197</c:v>
+                  <c:v>37.2863410465437</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>37.9470787434697</c:v>
+                  <c:v>37.3335527532908</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>38.0416543320442</c:v>
+                  <c:v>37.3818016196043</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>38.1396295542438</c:v>
+                  <c:v>37.4311104300867</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>38.2410816744691</c:v>
+                  <c:v>37.4815024698785</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>38.3460879571206</c:v>
+                  <c:v>37.533001535655</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>38.4547256665988</c:v>
+                  <c:v>37.5856319468627</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>38.5670720673044</c:v>
+                  <c:v>37.6394185572047</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>38.683204423638</c:v>
+                  <c:v>37.694386766377</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>38.8032</c:v>
+                  <c:v>37.7505625320626</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>38.9271360607911</c:v>
+                  <c:v>37.8079723821904</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>39.0550898704118</c:v>
+                  <c:v>37.8666434274618</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>39.1871386932628</c:v>
+                  <c:v>37.9266033741533</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>39.3233597937445</c:v>
+                  <c:v>37.9878805372007</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>39.4638304362575</c:v>
+                  <c:v>38.0505038535698</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>39.6086278852025</c:v>
+                  <c:v>38.1145028959215</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>39.75782940498</c:v>
+                  <c:v>38.1799078865769</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>39.9115122599905</c:v>
+                  <c:v>38.2467497117894</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>40.0697537146346</c:v>
+                  <c:v>38.3150599363298</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>40.232631033313</c:v>
+                  <c:v>38.3848708183925</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>40.4002214804261</c:v>
+                  <c:v>38.4562153248285</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>40.5726023203745</c:v>
+                  <c:v>38.5291271467136</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>40.7498508175589</c:v>
+                  <c:v>38.6036407152582</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>40.9320442363797</c:v>
+                  <c:v>38.6797912180671</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>41.1192598412375</c:v>
+                  <c:v>38.7576146157557</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>41.311574896533</c:v>
+                  <c:v>38.8371476589319</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>41.5090666666667</c:v>
+                  <c:v>38.9184279055512</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>41.7118124160391</c:v>
+                  <c:v>39.0014937386521</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>41.9198894090508</c:v>
+                  <c:v>39.0863843844823</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>42.1333749101025</c:v>
+                  <c:v>39.1731399310224</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>42.3523461835945</c:v>
+                  <c:v>39.2618013469164</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>42.5768804939277</c:v>
+                  <c:v>39.3524105008188</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>42.8070551055024</c:v>
+                  <c:v>39.4450101811658</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>43.0429472827193</c:v>
+                  <c:v>39.5396441163817</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>43.284634289979</c:v>
+                  <c:v>39.6363569955288</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>43.5321933916819</c:v>
+                  <c:v>39.7351944894106</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>43.7857018522288</c:v>
+                  <c:v>39.8362032721392</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>44.0452369360201</c:v>
+                  <c:v>39.9394310431766</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>44.3108759074564</c:v>
+                  <c:v>40.0449265498589</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>44.5826960309383</c:v>
+                  <c:v>40.1527396104175</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>44.8607745708664</c:v>
+                  <c:v>40.2629211375037</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>45.1451887916412</c:v>
+                  <c:v>40.3755231622321</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>45.4360159576634</c:v>
+                  <c:v>40.4905988587508</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>45.7333333333333</c:v>
+                  <c:v>40.6082025693518</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>46.0372181830518</c:v>
+                  <c:v>40.7283898301335</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>46.3477477712192</c:v>
+                  <c:v>40.8512173972264</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>46.6649993622363</c:v>
+                  <c:v>40.9767432735949</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>46.9890502205034</c:v>
+                  <c:v>41.1050267364284</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>47.3199776104213</c:v>
+                  <c:v>41.2361283651334</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>47.6578587963905</c:v>
+                  <c:v>41.3701100699416</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>48.0027710428116</c:v>
+                  <c:v>41.507035121145</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>48.3547916140851</c:v>
+                  <c:v>41.6469681789749</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>48.7139977746116</c:v>
+                  <c:v>41.7899753241359</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>49.0804667887916</c:v>
+                  <c:v>41.9361240890115</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>49.4542759210258</c:v>
+                  <c:v>42.0854834895547</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>49.8355024357148</c:v>
+                  <c:v>42.23812405788</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>50.224223597259</c:v>
+                  <c:v>42.3941178755702</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>50.620516670059</c:v>
+                  <c:v>42.5535386077159</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>51.0244589185155</c:v>
+                  <c:v>42.7164615377026</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>51.436127607029</c:v>
+                  <c:v>42.8829636027612</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>51.8556</c:v>
+                  <c:v>43.053123430301</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>52.2829533618292</c:v>
+                  <c:v>43.2270213750392</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>52.718264956917</c:v>
+                  <c:v>43.4047395569474</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>53.1616120496642</c:v>
+                  <c:v>43.5863619000307</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>53.6130719044711</c:v>
+                  <c:v>43.7719741719598</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>54.0727217857385</c:v>
+                  <c:v>43.9616640245728</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>54.5406389578669</c:v>
+                  <c:v>44.1555210352668</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>55.0169006852568</c:v>
+                  <c:v>44.3536367492999</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>55.5015842323089</c:v>
+                  <c:v>44.5561047230209</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>55.9947668634236</c:v>
+                  <c:v>44.76302056805</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>56.4965258430016</c:v>
+                  <c:v>44.9744819964291</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>57.0069384354434</c:v>
+                  <c:v>45.1905888667651</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>57.5260819051496</c:v>
+                  <c:v>45.4114432313857</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>58.0540335165208</c:v>
+                  <c:v>45.6371493845316</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>58.5908705339575</c:v>
+                  <c:v>45.8678139116078</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>59.1366702218604</c:v>
+                  <c:v>46.1035457395164</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>59.6915098446299</c:v>
+                  <c:v>46.3444561880951</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>60.2554666666667</c:v>
+                  <c:v>46.5906590226859</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>60.8286179523713</c:v>
+                  <c:v>46.842270507859</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>61.4110409661442</c:v>
+                  <c:v>47.0994094623157</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>62.0028129723862</c:v>
+                  <c:v>47.3621973149991</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>62.6040112354977</c:v>
+                  <c:v>47.630758162436</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>63.2147130198792</c:v>
+                  <c:v>47.9052188273395</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>63.8349955899315</c:v>
+                  <c:v>48.1857089184983</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>64.464936210055</c:v>
+                  <c:v>48.472360891982</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>65.1046121446503</c:v>
+                  <c:v>48.7653101136914</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>65.7541006581179</c:v>
+                  <c:v>49.0646949232817</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>66.4134790148585</c:v>
+                  <c:v>49.3706566994912</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>67.0828244792727</c:v>
+                  <c:v>49.6833399269049</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>67.7622143157609</c:v>
+                  <c:v>50.002892264184</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>68.4517257887238</c:v>
+                  <c:v>50.3294646137953</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>69.1514361625619</c:v>
+                  <c:v>50.6632111932718</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>69.8614227016758</c:v>
+                  <c:v>51.0042896080393</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>70.5817626704661</c:v>
+                  <c:v>51.3528609258421</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>71.3125333333333</c:v>
+                  <c:v>51.7090897528043</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>72.0538119546781</c:v>
+                  <c:v>52.073144311162</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>72.8056757989009</c:v>
+                  <c:v>52.445196518703</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>73.5682021304023</c:v>
+                  <c:v>52.8254220699517</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>74.341468213583</c:v>
+                  <c:v>53.2140005191373</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>75.1255513128435</c:v>
+                  <c:v>53.611115364985</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>75.9205286925843</c:v>
+                  <c:v>54.0169541373697</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>76.7264776172061</c:v>
+                  <c:v>54.4317084858735</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>77.5434753511093</c:v>
+                  <c:v>54.8555742702883</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>78.3715991586946</c:v>
+                  <c:v>55.288751653107</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>79.2109263043626</c:v>
+                  <c:v>55.7314451940466</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>80.0615340525137</c:v>
+                  <c:v>56.1838639466471</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>80.9234996675487</c:v>
+                  <c:v>56.6462215569934</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>81.796900413868</c:v>
+                  <c:v>57.1187363646057</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>82.6818135558722</c:v>
+                  <c:v>57.6016315055457</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>83.5783163579619</c:v>
+                  <c:v>58.0951350177885</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>84.4864860845376</c:v>
+                  <c:v>58.5994799489095</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>85.4064</c:v>
+                  <c:v>59.1149044661362</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>86.3381353687496</c:v>
+                  <c:v>59.6416519688183</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>87.2817694551869</c:v>
+                  <c:v>60.1799712033685</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>88.2373795237126</c:v>
+                  <c:v>60.7301163807278</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>89.2050428387272</c:v>
+                  <c:v>61.2923472964123</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>90.1848366646313</c:v>
+                  <c:v>61.8669294531964</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>91.1768382658254</c:v>
+                  <c:v>62.4541341864913</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>92.1811249067101</c:v>
+                  <c:v>63.0542387924779</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>93.197773851686</c:v>
+                  <c:v>63.667526659055</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>94.2268623651537</c:v>
+                  <c:v>64.2942873996634</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>95.2684677115137</c:v>
+                  <c:v>64.9348169900504</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>96.3226671551666</c:v>
+                  <c:v>65.5894179080389</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>97.3895379605129</c:v>
+                  <c:v>66.2583992763665</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>98.4691573919533</c:v>
+                  <c:v>66.9420770086626</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>99.5616027138883</c:v>
+                  <c:v>67.6407739586333</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>100.666951190719</c:v>
+                  <c:v>68.3548200725219</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>101.785280086844</c:v>
+                  <c:v>69.0845525449205</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>102.916666666667</c:v>
+                  <c:v>69.8303159780033</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>104.061188194586</c:v>
+                  <c:v>70.5924625442583</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>105.218921935002</c:v>
+                  <c:v>71.3713521527944</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>106.389945152317</c:v>
+                  <c:v>72.1673526193011</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>107.57433511093</c:v>
+                  <c:v>72.9808398397427</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>108.772169075243</c:v>
+                  <c:v>73.8121979678679</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>109.983524309655</c:v>
+                  <c:v>74.661819596619</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>111.208478078567</c:v>
+                  <c:v>75.5301059435266</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>112.44710764638</c:v>
+                  <c:v>76.4174670401766</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>113.699490277495</c:v>
+                  <c:v>77.3243219258398</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>114.965703236312</c:v>
+                  <c:v>78.2510988453554</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>116.245823787231</c:v>
+                  <c:v>79.1982354513611</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>117.539929194654</c:v>
+                  <c:v>80.1661790109667</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>118.84809672298</c:v>
+                  <c:v>81.1553866169665</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>120.17040363661</c:v>
+                  <c:v>82.1663254036936</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>121.506927199946</c:v>
+                  <c:v>83.1994727676146</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>122.857744677387</c:v>
+                  <c:v>84.2553165927709</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>124.222933333333</c:v>
+                  <c:v>85.3343554811729</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>125.602570432187</c:v>
+                  <c:v>86.4370989882549</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>126.996733238347</c:v>
+                  <c:v>87.5640678635032</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>128.405499016216</c:v>
+                  <c:v>88.7157942963698</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>129.828945030192</c:v>
+                  <c:v>89.892822167589</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>131.267148544677</c:v>
+                  <c:v>91.0957073060141</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>132.720186824072</c:v>
+                  <c:v>92.3250177510975</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>134.188137132777</c:v>
+                  <c:v>93.5813340211361</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>135.671076735192</c:v>
+                  <c:v>94.8652493874103</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>137.169082895719</c:v>
+                  <c:v>96.1773701543443</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>138.682232878757</c:v>
+                  <c:v>97.5183159458225</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>140.210603948708</c:v>
+                  <c:v>98.8887199977947</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>141.754273369971</c:v>
+                  <c:v>100.289229457309</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>143.313318406948</c:v>
+                  <c:v>101.720505688117</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>144.887816324038</c:v>
+                  <c:v>103.183224582986</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>146.477844385643</c:v>
+                  <c:v>104.67807688288</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>148.083479856164</c:v>
+                  <c:v>106.205768503148</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>149.7048</c:v>
+                  <c:v>107.767020866878</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>151.341882081552</c:v>
+                  <c:v>109.362571245576</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>152.994803365222</c:v>
+                  <c:v>110.993173107328</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>154.663641115408</c:v>
+                  <c:v>112.659596472612</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>156.348472596513</c:v>
+                  <c:v>114.362628277924</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>158.049375072936</c:v>
+                  <c:v>116.103072747393</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>159.766425809078</c:v>
+                  <c:v>117.881751772564</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>161.49970206934</c:v>
+                  <c:v>119.699505300516</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>163.249281118122</c:v>
+                  <c:v>121.557191730514</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>165.015240219825</c:v>
+                  <c:v>123.455688319371</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>166.797656638849</c:v>
+                  <c:v>125.395891595714</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>168.596607639596</c:v>
+                  <c:v>127.378717783355</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>170.412170486464</c:v>
+                  <c:v>129.405103233958</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>172.244422443856</c:v>
+                  <c:v>131.476004869216</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>174.093440776172</c:v>
+                  <c:v>133.592400632735</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>175.959302747812</c:v>
+                  <c:v>135.755289951853</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>177.842085623177</c:v>
+                  <c:v>137.965694209595</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>179.741866666667</c:v>
+                  <c:v>140.22465722701</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>181.658723142683</c:v>
+                  <c:v>142.533245756086</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>183.592732315625</c:v>
+                  <c:v>144.892549983511</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>185.543971449895</c:v>
+                  <c:v>147.303684045489</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>187.512517809892</c:v>
+                  <c:v>149.767786553868</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>189.498448660018</c:v>
+                  <c:v>152.286021133832</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>191.501841264672</c:v>
+                  <c:v>154.859576973397</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>193.522772888256</c:v>
+                  <c:v>157.489669384984</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>195.561320795169</c:v>
+                  <c:v>160.177540379327</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>197.617562249813</c:v>
+                  <c:v>162.924459251987</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>199.691574516589</c:v>
+                  <c:v>165.731723182754</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>201.783434859895</c:v>
+                  <c:v>168.600657848218</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>203.893220544135</c:v>
+                  <c:v>171.532618047788</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>206.021008833706</c:v>
+                  <c:v>174.528988343475</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>208.166876993012</c:v>
+                  <c:v>177.591183713723</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>210.330902286451</c:v>
+                  <c:v>180.720650221606</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>212.513161978425</c:v>
+                  <c:v>183.918865697705</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>214.713733333333</c:v>
+                  <c:v>187.18734043798</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>216.932693615578</c:v>
+                  <c:v>190.527617916985</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>219.170120089558</c:v>
+                  <c:v>193.941275516741</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>221.426090019676</c:v>
+                  <c:v>197.429925271623</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>223.70068067033</c:v>
+                  <c:v>200.995214629616</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>225.993969305923</c:v>
+                  <c:v>204.638827230286</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>228.306033190854</c:v>
+                  <c:v>208.362483699853</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>230.636949589524</c:v>
+                  <c:v>212.167942463716</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>232.986795766334</c:v>
+                  <c:v>216.057000576842</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>235.355648985684</c:v>
+                  <c:v>220.031494572388</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>237.743586511975</c:v>
+                  <c:v>224.093301328969</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>240.150685609607</c:v>
+                  <c:v>228.244338956978</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>242.577023542981</c:v>
+                  <c:v>232.486567704377</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>245.022677576498</c:v>
+                  <c:v>236.821990882386</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>247.487724974557</c:v>
+                  <c:v>241.252655811509</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>249.97224300156</c:v>
+                  <c:v>245.780654788341</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>252.476308921908</c:v>
+                  <c:v>250.408126073617</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>255</c:v>
+                  <c:v>255.137254901961</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3672,11 +3672,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="87796409"/>
-        <c:axId val="53096067"/>
+        <c:axId val="11242264"/>
+        <c:axId val="48795442"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87796409"/>
+        <c:axId val="11242264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3704,14 +3704,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53096067"/>
+        <c:crossAx val="48795442"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53096067"/>
+        <c:axId val="48795442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3726,7 +3726,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3748,7 +3748,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87796409"/>
+        <c:crossAx val="11242264"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3872,8 +3872,8 @@
   </sheetPr>
   <dimension ref="B1:D262"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7273,8 +7273,8 @@
   </sheetPr>
   <dimension ref="A1:D263"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E250" activeCellId="0" sqref="E250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>